<commit_message>
Added kinematics C script and some other stuff
Kinematics script, written for now as a C program that outputs the desired codes for the SSC-32 based on X,Y,Z positions.
</commit_message>
<xml_diff>
--- a/PCB/Provisional_BOM.xlsx
+++ b/PCB/Provisional_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jimbo\Documents\GitHub\GDIP_ROBOT\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC25389A-8649-49F5-8A13-1ECA48AB0001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D851BD-70D4-441A-AB39-B3356933432A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{CEE32223-6BE1-4461-9294-2E2B54D3A86B}"/>
   </bookViews>
@@ -107,19 +107,22 @@
     <t>https://www.mouser.co.uk/ProductDetail/Espressif-Systems/ESP32-S2-DevKitC-1RU?qs=pBJMDPsKWf1wWYxkgQUBfQ%3D%3D&amp;mgh=1&amp;vip=1&amp;gclid=CjwKCAiA7IGcBhA8EiwAFfUDsYRj10h3izk5vQ4UWmTe7Dn7_zCRgf5sXVQpd2JwSykeqy0EkNWQARoC7jYQAvD_BwE</t>
   </si>
   <si>
-    <t>PiHut</t>
-  </si>
-  <si>
-    <t>https://thepihut.com/products/5v-electromagnet-10-kg-holding-force</t>
-  </si>
-  <si>
-    <t>Electromagnet 5V 10kg</t>
+    <t>Electromagnet 5V 25kg</t>
+  </si>
+  <si>
+    <t>Farnell</t>
+  </si>
+  <si>
+    <t>https://uk.farnell.com/dfrobot/dfr0800/electromagnetic-lock-5v-25kg/dp/3769906?gclid=Cj0KCQiAm5ycBhCXARIsAPldzoXpMsX7goYBt_3BHIXdxOR6pkPWgVRATAw-KLtvC3f8cBxiMN1z8-caApd1EALw_wcB&amp;mckv=_dc|pcrid||plid||kword||match||slid||product|3769906|pgrid||ptaid|&amp;CMP=KNC-GUK-GEN-SHOPPING-SMART-PMAX-Medium_ROAS-Test958&amp;gross_price=true</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -158,9 +161,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -476,196 +480,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73250971-4E20-4FF7-96ED-56803F45581C}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="81.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="5" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="81.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="B2">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" s="2">
+        <v>12.21</v>
+      </c>
+      <c r="D2" s="2">
+        <v>14.651999999999999</v>
+      </c>
+      <c r="E2" s="2">
+        <f>B2*D2</f>
+        <v>29.303999999999998</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G4" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
         <v>12</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
         <v>12</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
         <v>3</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
         <v>3</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
         <v>12</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>10.54</v>
+      </c>
+      <c r="E11" s="2">
+        <v>10.54</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F1" r:id="rId1" display="https://www.digikey.co.uk/en/products/detail/adafruit-industries-llc/324/5022791?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax:%20Smart%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;productid=5022791&amp;gclid=CjwKCAiA7IGcBhA8EiwAFfUDsTNRLcWA6HjCHboznJs4vu9jdAmZ9ACY08ebfRRH66cpmNJiw-DjmxoCTKYQAvD_BwE" xr:uid="{E945F1B5-9669-4070-83CF-F5B760C17510}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{FB947886-B513-46CA-B2CF-7C67E90770F4}"/>
+    <hyperlink ref="H2" r:id="rId1" display="https://www.digikey.co.uk/en/products/detail/adafruit-industries-llc/324/5022791?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax:%20Smart%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;productid=5022791&amp;gclid=CjwKCAiA7IGcBhA8EiwAFfUDsTNRLcWA6HjCHboznJs4vu9jdAmZ9ACY08ebfRRH66cpmNJiw-DjmxoCTKYQAvD_BwE" xr:uid="{E945F1B5-9669-4070-83CF-F5B760C17510}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{FB947886-B513-46CA-B2CF-7C67E90770F4}"/>
+    <hyperlink ref="H11" r:id="rId3" display="https://uk.farnell.com/dfrobot/dfr0800/electromagnetic-lock-5v-25kg/dp/3769906?gclid=Cj0KCQiAm5ycBhCXARIsAPldzoXpMsX7goYBt_3BHIXdxOR6pkPWgVRATAw-KLtvC3f8cBxiMN1z8-caApd1EALw_wcB&amp;mckv=_dc|pcrid||plid||kword||match||slid||product|3769906|pgrid||ptaid|&amp;CMP=KNC-GUK-GEN-SHOPPING-SMART-PMAX-Medium_ROAS-Test958&amp;gross_price=true" xr:uid="{9DA76943-663A-4ACC-B405-7C02FC244042}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>